<commit_message>
Updated project journal time
</commit_message>
<xml_diff>
--- a/Project Journal.xlsx
+++ b/Project Journal.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t xml:space="preserve">Name: </t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Please update your tab on this journal to keep track of the time spent working on the project</t>
+  </si>
+  <si>
+    <t>Added new header files. Implemented part of Database.h</t>
   </si>
 </sst>
 </file>
@@ -302,12 +305,6 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -319,9 +316,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -345,6 +339,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -674,45 +677,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="6" t="str">
+      <c r="A2" s="4" t="str">
         <f>Jesse!B1</f>
         <v>Jesse Hankins</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="5">
         <f>(Jesse!C2)/60</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="6" t="str">
+      <c r="A3" s="4" t="str">
         <f>Deanna!B1</f>
         <v>Deanna Tatum</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <f>(Deanna!C2)/60</f>
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="17" t="str">
+      <c r="A4" s="14" t="str">
         <f>Kyle!B1</f>
         <v>Kyle Meystedt</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="13">
         <f>(Kyle!C2)/60</f>
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="15" t="s">
         <v>10</v>
       </c>
     </row>
@@ -723,58 +726,69 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220D8536-BF03-4DF5-B3B5-AB5FD1A42F84}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="G14" sqref="G13:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.19921875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.3984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.59765625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="10.19921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.59765625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="12">
+      <c r="B2" s="18"/>
+      <c r="C2" s="9">
         <f>SUM(B4:B200)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="6">
+        <v>43028</v>
+      </c>
+      <c r="B4" s="3">
         <v>180</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="9">
-        <v>43028</v>
-      </c>
-      <c r="B4" s="5">
-        <v>180</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="6">
+        <v>43038</v>
+      </c>
+      <c r="B5" s="3">
+        <v>60</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -797,49 +811,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.19921875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.3984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.59765625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="10.19921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.59765625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="12">
+      <c r="B2" s="18"/>
+      <c r="C2" s="9">
         <f>SUM(B4:B200)</f>
         <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>43028</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>180</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
     </row>
@@ -863,49 +877,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.19921875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.3984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.59765625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="10.19921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.59765625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="12">
+      <c r="B2" s="18"/>
+      <c r="C2" s="9">
         <f>SUM(B4:B200)</f>
         <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>43028</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>180</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Project report, and input file for testing. Completed Room explicit constructor.
</commit_message>
<xml_diff>
--- a/Project Journal.xlsx
+++ b/Project Journal.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t xml:space="preserve">Name: </t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>Added new header files. Implemented part of Database.h</t>
+  </si>
+  <si>
+    <t>10/3102017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completed Room explicit constructor. Added input file for testing. </t>
   </si>
 </sst>
 </file>
@@ -691,7 +697,7 @@
       </c>
       <c r="B2" s="5">
         <f>(Jesse!C2)/60</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -726,10 +732,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220D8536-BF03-4DF5-B3B5-AB5FD1A42F84}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G13:G14"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -755,7 +761,7 @@
       <c r="B2" s="18"/>
       <c r="C2" s="9">
         <f>SUM(B4:B200)</f>
-        <v>240</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -789,6 +795,17 @@
       </c>
       <c r="C5" s="11" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3">
+        <v>120</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added BuildingInfo.txt to explain input file formatting. Corrected location of stairs in roomID f2r410. Added setSymbol function in Objects.h. Completed stairs symbol assignment in Rooms.h. Added basic menu and probability functions in main. Changed definitions from in-line to prototype in header and definition in separate cpp for Objects and Rooms. Added notation sections to headers of Objects.h and Rooms.h.
</commit_message>
<xml_diff>
--- a/Project Journal.xlsx
+++ b/Project Journal.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -65,10 +65,19 @@
     <t>Added new header files. Implemented part of Database.h</t>
   </si>
   <si>
-    <t>10/3102017</t>
-  </si>
-  <si>
     <t xml:space="preserve">Completed Room explicit constructor. Added input file for testing. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added data member 'next' and function 'setNext' to Object superclass. 
+Edited Object assignment in Rooms.h to account for next data members. 
+Created a test building consisting only of rooms, stairs, and doors that has two floors and a basement.
+Added BuildingInfo.txt to explain input file formatting.
+Corrected location of stairs in roomID f2r410. 
+Added setSymbol function in Objects.h. 
+Completed stairs symbol assignment in Rooms.h. 
+Added basic menu and probability functions in main. 
+Changed definitions from in-line to prototype in header and definition in separate cpp for Objects and Rooms.
+Added notation sections to headers of Objects.h and Rooms.h. </t>
   </si>
 </sst>
 </file>
@@ -697,7 +706,7 @@
       </c>
       <c r="B2" s="5">
         <f>(Jesse!C2)/60</f>
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -732,10 +741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220D8536-BF03-4DF5-B3B5-AB5FD1A42F84}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -761,7 +770,7 @@
       <c r="B2" s="18"/>
       <c r="C2" s="9">
         <f>SUM(B4:B200)</f>
-        <v>360</v>
+        <v>660</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -798,13 +807,24 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="6" t="s">
-        <v>12</v>
+      <c r="A6" s="6">
+        <v>43039</v>
       </c>
       <c r="B6" s="3">
         <v>120</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="270.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="6">
+        <v>43059</v>
+      </c>
+      <c r="B7" s="3">
+        <v>300</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added data member 'shift' and functions 'setShift', 'getShift', and 'getNext' to Object superclass. Edited Object assignment in Rooms.h to account for shift data members. Added shift values to room files for Doors and Windows. Added description for 'shift' in BuildingInfo.txt. Removed overloaded output operator for class Rooms. Added function 'displayRoom' to class Rooms.
</commit_message>
<xml_diff>
--- a/Project Journal.xlsx
+++ b/Project Journal.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10988" xr2:uid="{551A70F0-0B56-434D-A545-C690E3630407}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10988" activeTab="1" xr2:uid="{551A70F0-0B56-434D-A545-C690E3630407}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t xml:space="preserve">Name: </t>
   </si>
@@ -78,6 +78,14 @@
 Added basic menu and probability functions in main. 
 Changed definitions from in-line to prototype in header and definition in separate cpp for Objects and Rooms.
 Added notation sections to headers of Objects.h and Rooms.h. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added data member 'shift' and functions 'setShift', 'getShift', and 'getNext' to Object superclass. 
+Edited Object assignment in Rooms.h to account for shift data members.
+Added shift values to room files for Doors and Windows. 
+Added description for 'shift' in BuildingInfo.txt.
+Removed overloaded output operator for class Rooms. 
+Added function 'displayRoom' to class Rooms. </t>
   </si>
 </sst>
 </file>
@@ -680,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DCFF5D7-D7F8-409B-A3B4-F198DB463BCD}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -706,7 +714,7 @@
       </c>
       <c r="B2" s="5">
         <f>(Jesse!C2)/60</f>
-        <v>11</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -741,9 +749,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220D8536-BF03-4DF5-B3B5-AB5FD1A42F84}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -770,7 +778,7 @@
       <c r="B2" s="18"/>
       <c r="C2" s="9">
         <f>SUM(B4:B200)</f>
-        <v>660</v>
+        <v>750</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -826,6 +834,17 @@
       </c>
       <c r="C7" s="11" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="156.75" x14ac:dyDescent="0.45">
+      <c r="A8" s="6">
+        <v>43068</v>
+      </c>
+      <c r="B8" s="3">
+        <v>90</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added getObjects() to Rooms.h to return the vector of objects. Created Building.h, and Building.cpp as a Tree-like structure. Removed Maps.h and Database.h.
</commit_message>
<xml_diff>
--- a/Project Journal.xlsx
+++ b/Project Journal.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10988" activeTab="1" xr2:uid="{551A70F0-0B56-434D-A545-C690E3630407}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10988" xr2:uid="{551A70F0-0B56-434D-A545-C690E3630407}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t xml:space="preserve">Name: </t>
   </si>
@@ -86,6 +86,10 @@
 Added description for 'shift' in BuildingInfo.txt.
 Removed overloaded output operator for class Rooms. 
 Added function 'displayRoom' to class Rooms. </t>
+  </si>
+  <si>
+    <t>Added function getObjects() to Rooms.h to return the vector of objects. 
+Created Building.h, and Building.cpp as a Tree-like structure.</t>
   </si>
 </sst>
 </file>
@@ -688,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DCFF5D7-D7F8-409B-A3B4-F198DB463BCD}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -714,7 +718,7 @@
       </c>
       <c r="B2" s="5">
         <f>(Jesse!C2)/60</f>
-        <v>12.5</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -749,10 +753,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220D8536-BF03-4DF5-B3B5-AB5FD1A42F84}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -778,7 +782,7 @@
       <c r="B2" s="18"/>
       <c r="C2" s="9">
         <f>SUM(B4:B200)</f>
-        <v>750</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -845,6 +849,17 @@
       </c>
       <c r="C8" s="11" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+      <c r="A9" s="6">
+        <v>43071</v>
+      </c>
+      <c r="B9" s="3">
+        <v>360</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functions getRoot() and findNext() to Building.h to premit traversal. Added data members, inheretance, and Deploy() function to States.h to handle traversal/generation. Added comments for coding suggestions in States.h
</commit_message>
<xml_diff>
--- a/Project Journal.xlsx
+++ b/Project Journal.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t xml:space="preserve">Name: </t>
   </si>
@@ -90,6 +90,11 @@
   <si>
     <t>Added function getObjects() to Rooms.h to return the vector of objects. 
 Created Building.h, and Building.cpp as a Tree-like structure.</t>
+  </si>
+  <si>
+    <t>Added functions getRoot() and findNext() to Building.h to premit traversal. 
+Added data members, inheretance, and Deploy() function to States.h to handle traversal/generation. 
+Added comments for coding suggestions in States.h</t>
   </si>
 </sst>
 </file>
@@ -718,7 +723,7 @@
       </c>
       <c r="B2" s="5">
         <f>(Jesse!C2)/60</f>
-        <v>18.5</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -753,10 +758,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220D8536-BF03-4DF5-B3B5-AB5FD1A42F84}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -782,7 +787,7 @@
       <c r="B2" s="18"/>
       <c r="C2" s="9">
         <f>SUM(B4:B200)</f>
-        <v>1110</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -860,6 +865,17 @@
       </c>
       <c r="C9" s="11" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A10" s="6">
+        <v>43074</v>
+      </c>
+      <c r="B10" s="3">
+        <v>180</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>